<commit_message>
Task            : Sprint Planning Sheet update Files Added     : AlkeshSrivastav.xlsx Files Deleted   : none Description     : Updated the hours burnt column in the sprint planning sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
+++ b/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>T6</t>
-  </si>
-  <si>
-    <t>Connect the JRXML file to Jasper Report template.</t>
   </si>
   <si>
     <t>T7</t>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t>SSDMS 41</t>
+  </si>
+  <si>
+    <t>Complile the JRXML file to Jasper Report template.</t>
   </si>
 </sst>
 </file>
@@ -523,30 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -556,6 +532,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,17 +878,17 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="26">
+      <c r="A2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="30">
         <v>14.5</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -898,13 +898,13 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -918,13 +918,13 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="11">
         <v>2</v>
@@ -937,13 +937,13 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5">
         <v>2</v>
@@ -957,13 +957,13 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="11">
         <v>1.5</v>
@@ -977,13 +977,13 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -1005,13 +1005,13 @@
       <c r="O7" s="17"/>
     </row>
     <row r="8" spans="1:15" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="11">
         <v>2</v>
@@ -1033,13 +1033,13 @@
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1061,13 +1061,13 @@
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="11">
         <v>2</v>
@@ -1089,13 +1089,13 @@
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -1117,13 +1117,13 @@
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>20</v>
       </c>
       <c r="E12" s="11">
         <v>0.5</v>
@@ -1145,13 +1145,13 @@
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5">
         <v>0.5</v>
@@ -1174,12 +1174,12 @@
     </row>
     <row r="16" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="D16" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="120" x14ac:dyDescent="0.25">
       <c r="D17" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:CS16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,17 +1234,17 @@
       </c>
     </row>
     <row r="2" spans="1:97" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="28">
+      <c r="A2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="32">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1254,8 +1254,8 @@
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
@@ -1266,41 +1266,41 @@
         <v>3</v>
       </c>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="7">
         <v>3</v>
@@ -1314,13 +1314,13 @@
       </c>
     </row>
     <row r="6" spans="1:97" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -1424,13 +1424,13 @@
       <c r="CS6" s="17"/>
     </row>
     <row r="7" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1527,13 +1527,13 @@
       <c r="CS7" s="17"/>
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1630,13 +1630,13 @@
       <c r="CS8" s="17"/>
     </row>
     <row r="9" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -1740,13 +1740,13 @@
       <c r="CS9" s="17"/>
     </row>
     <row r="10" spans="1:97" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1850,13 +1850,13 @@
       <c r="CS10" s="17"/>
     </row>
     <row r="11" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
@@ -1960,13 +1960,13 @@
       <c r="CS11" s="17"/>
     </row>
     <row r="12" spans="1:97" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4">
         <v>2</v>
@@ -2070,20 +2070,20 @@
       <c r="CS12" s="17"/>
     </row>
     <row r="15" spans="1:97" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="32" t="s">
+      <c r="A15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:97" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="33"/>
-    </row>
-    <row r="16" spans="1:97" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="33"/>
+      <c r="E16" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Task            : Sprint Planning Sheet update Files Added     : AlkeshSrivastav.xlsx Files Deleted   : none Description     : Updated the hours burnt column in the sprint planning sheet and added a Status column
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
+++ b/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Story ID</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>T5</t>
-  </si>
-  <si>
-    <t>Create a JRXML file using iReport Designer.</t>
   </si>
   <si>
     <t>T6</t>
@@ -313,6 +310,21 @@
   <si>
     <t>Complile the JRXML file to Jasper Report template.</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Create a JRXML file using JasperSoft studio.</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
 </sst>
 </file>
 
@@ -344,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +423,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -474,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +586,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,9 +889,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -876,10 +914,13 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="H1" s="40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="30">
         <v>14.5</v>
@@ -888,7 +929,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -896,15 +937,18 @@
         <f t="shared" ref="G2:G13" si="0">E2-F2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H2" s="39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="30"/>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -916,15 +960,18 @@
         <f>E3-F3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="11">
         <v>2</v>
@@ -935,15 +982,18 @@
       <c r="G4" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="30"/>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5">
         <v>2</v>
@@ -955,15 +1005,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H5" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="30"/>
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="11">
         <v>1.5</v>
@@ -975,15 +1028,18 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -995,7 +1051,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -1003,15 +1061,18 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+    </row>
+    <row r="8" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="30"/>
       <c r="C8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="11">
         <v>2</v>
@@ -1023,7 +1084,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -1031,15 +1094,18 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
-    </row>
-    <row r="9" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+    </row>
+    <row r="9" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
       <c r="B9" s="30"/>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1051,7 +1117,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -1059,15 +1127,18 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
-    </row>
-    <row r="10" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+    </row>
+    <row r="10" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="30"/>
       <c r="C10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="11">
         <v>2</v>
@@ -1079,7 +1150,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1087,15 +1160,18 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+    </row>
+    <row r="11" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="30"/>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -1107,7 +1183,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -1115,15 +1193,18 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="30"/>
       <c r="C12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="E12" s="11">
         <v>0.5</v>
@@ -1135,7 +1216,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -1143,15 +1226,18 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+    </row>
+    <row r="13" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
       <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="5">
         <v>0.5</v>
@@ -1163,7 +1249,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -1171,15 +1259,23 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
-    </row>
-    <row r="16" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G14" s="37">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="D16" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="120" x14ac:dyDescent="0.25">
       <c r="D17" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1196,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,6 +1304,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.25">
@@ -1232,25 +1329,31 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="40" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" spans="1:97" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="32">
         <v>18</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4">
         <f t="shared" ref="G2:G12" si="0">E2-F2</f>
         <v>0</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.25">
@@ -1260,7 +1363,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E3" s="7">
         <v>3</v>
@@ -1271,6 +1374,9 @@
       <c r="G3" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.25">
@@ -1280,7 +1386,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -1291,16 +1397,19 @@
       <c r="G4" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="32"/>
       <c r="C5" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7">
         <v>3</v>
@@ -1311,6 +1420,9 @@
       <c r="G5" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:97" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -1320,7 +1432,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -1332,7 +1444,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
@@ -1427,10 +1541,10 @@
       <c r="A7" s="34"/>
       <c r="B7" s="32"/>
       <c r="C7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
@@ -1442,7 +1556,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -1537,10 +1653,10 @@
       <c r="A8" s="34"/>
       <c r="B8" s="32"/>
       <c r="C8" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
@@ -1552,7 +1668,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -1647,10 +1765,10 @@
       <c r="A9" s="34"/>
       <c r="B9" s="32"/>
       <c r="C9" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -1662,7 +1780,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -1757,10 +1877,10 @@
       <c r="A10" s="34"/>
       <c r="B10" s="32"/>
       <c r="C10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1772,7 +1892,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1867,10 +1989,10 @@
       <c r="A11" s="34"/>
       <c r="B11" s="32"/>
       <c r="C11" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
@@ -1882,7 +2004,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -1977,10 +2101,10 @@
       <c r="A12" s="35"/>
       <c r="B12" s="33"/>
       <c r="C12" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4">
         <v>2</v>
@@ -1992,7 +2116,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -2083,11 +2209,16 @@
       <c r="CR12" s="17"/>
       <c r="CS12" s="17"/>
     </row>
+    <row r="13" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="G13" s="37">
+        <v>13</v>
+      </c>
+    </row>
     <row r="15" spans="1:97" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="25"/>
     </row>
@@ -2095,7 +2226,7 @@
       <c r="A16" s="26"/>
       <c r="C16" s="25"/>
       <c r="D16" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="25"/>
     </row>

</xml_diff>

<commit_message>
Task            : Sprint Planning Sheet update Files Added     : AlkeshSrivastav.xlsx Files Deleted   : none Description     : Updated the hours burnt column
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
+++ b/TeamDetails/TasksBreakDown/AlkeshSrivastav.xlsx
@@ -563,36 +563,36 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,15 +914,15 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="35">
         <v>14.5</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -937,13 +937,13 @@
         <f t="shared" ref="G2:G13" si="0">E2-F2</f>
         <v>0</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
@@ -960,13 +960,13 @@
         <f>E3-F3</f>
         <v>1</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
@@ -982,13 +982,13 @@
       <c r="G4" s="11">
         <v>2</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1005,13 +1005,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
@@ -1028,13 +1028,13 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:18" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1051,7 +1051,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I7" s="17"/>
@@ -1066,8 +1066,8 @@
       <c r="R7" s="17"/>
     </row>
     <row r="8" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1084,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="17"/>
@@ -1099,8 +1099,8 @@
       <c r="R8" s="17"/>
     </row>
     <row r="9" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1117,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I9" s="17"/>
@@ -1132,8 +1132,8 @@
       <c r="R9" s="17"/>
     </row>
     <row r="10" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1150,7 +1150,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="17"/>
@@ -1165,8 +1165,8 @@
       <c r="R10" s="17"/>
     </row>
     <row r="11" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1183,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="17"/>
@@ -1198,8 +1198,8 @@
       <c r="R11" s="17"/>
     </row>
     <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1216,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I12" s="17"/>
@@ -1231,8 +1231,8 @@
       <c r="R12" s="17"/>
     </row>
     <row r="13" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1249,7 +1249,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I13" s="17"/>
@@ -1264,7 +1264,7 @@
       <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G14" s="37">
+      <c r="G14" s="29">
         <v>14.5</v>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
   <dimension ref="A1:CS16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,15 +1329,15 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:97" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="37">
         <v>18</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -1352,13 +1352,13 @@
         <f t="shared" ref="G2:G12" si="0">E2-F2</f>
         <v>0</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
@@ -1375,13 +1375,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
@@ -1398,13 +1398,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
@@ -1415,19 +1415,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>50</v>
+        <f>E5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:97" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1438,14 +1438,14 @@
         <v>2</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>50</v>
+        <f>E6-F6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>49</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -1538,8 +1538,8 @@
       <c r="CS6" s="17"/>
     </row>
     <row r="7" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1556,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I7" s="17"/>
@@ -1650,8 +1650,8 @@
       <c r="CS7" s="17"/>
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
@@ -1668,7 +1668,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="17"/>
@@ -1762,8 +1762,8 @@
       <c r="CS8" s="17"/>
     </row>
     <row r="9" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="14" t="s">
         <v>14</v>
       </c>
@@ -1780,7 +1780,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I9" s="17"/>
@@ -1874,8 +1874,8 @@
       <c r="CS9" s="17"/>
     </row>
     <row r="10" spans="1:97" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="15" t="s">
         <v>15</v>
       </c>
@@ -1892,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="17"/>
@@ -1986,8 +1986,8 @@
       <c r="CS10" s="17"/>
     </row>
     <row r="11" spans="1:97" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="14" t="s">
         <v>27</v>
       </c>
@@ -2004,7 +2004,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="17"/>
@@ -2098,8 +2098,8 @@
       <c r="CS11" s="17"/>
     </row>
     <row r="12" spans="1:97" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="16" t="s">
         <v>17</v>
       </c>
@@ -2116,7 +2116,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I12" s="17"/>
@@ -2210,8 +2210,8 @@
       <c r="CS12" s="17"/>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="G13" s="37">
-        <v>13</v>
+      <c r="G13" s="29">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:97" ht="60" x14ac:dyDescent="0.25">

</xml_diff>